<commit_message>
ParkSS - DB and insert dll new registers
</commit_message>
<xml_diff>
--- a/ParkDACE/files/Campus_2_B_Park2.xlsx
+++ b/ParkDACE/files/Campus_2_B_Park2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DestruidorPT\source\repos\IS_Project\ParkDACE\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andre\Desktop\Project_IS\IS_Project\ParkDACE\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{1FD23A32-49DC-40EF-BEFE-D9A258202EA3}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{40CBD845-79A0-49D7-81CD-F7BC0C7E2EEE}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17490" windowHeight="7980" xr2:uid="{E9C09612-09AF-3E4B-99D2-8B8D15F60D70}"/>
   </bookViews>
@@ -36,36 +36,6 @@
     <t>Updated Data:</t>
   </si>
   <si>
-    <t>A-1</t>
-  </si>
-  <si>
-    <t>A-2</t>
-  </si>
-  <si>
-    <t>A-3</t>
-  </si>
-  <si>
-    <t>A-4</t>
-  </si>
-  <si>
-    <t>A-5</t>
-  </si>
-  <si>
-    <t>A-6</t>
-  </si>
-  <si>
-    <t>A-7</t>
-  </si>
-  <si>
-    <t>A-8</t>
-  </si>
-  <si>
-    <t>A-9</t>
-  </si>
-  <si>
-    <t>A-10</t>
-  </si>
-  <si>
     <t>39.734859,-8.820784</t>
   </si>
   <si>
@@ -103,6 +73,36 @@
   </si>
   <si>
     <t>Campus_2_B_Park2</t>
+  </si>
+  <si>
+    <t>B-1</t>
+  </si>
+  <si>
+    <t>B-2</t>
+  </si>
+  <si>
+    <t>B-3</t>
+  </si>
+  <si>
+    <t>B-4</t>
+  </si>
+  <si>
+    <t>B-5</t>
+  </si>
+  <si>
+    <t>B-6</t>
+  </si>
+  <si>
+    <t>B-7</t>
+  </si>
+  <si>
+    <t>B-8</t>
+  </si>
+  <si>
+    <t>B-9</t>
+  </si>
+  <si>
+    <t>B-10</t>
   </si>
 </sst>
 </file>
@@ -469,8 +469,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0941C8BF-080F-0841-8CAE-654BE7571C9E}">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="173" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" zoomScale="173" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -484,7 +484,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -505,93 +505,94 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
         <v>3</v>
-      </c>
-      <c r="B6" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
         <v>4</v>
-      </c>
-      <c r="B7" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
         <v>5</v>
-      </c>
-      <c r="B8" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="B10" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="B12" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="B13" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="B14" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="B15" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>